<commit_message>
Energy Balance and Energy Consumption improvements
</commit_message>
<xml_diff>
--- a/Structure/1 - Whole System/EnBalance.xlsx
+++ b/Structure/1 - Whole System/EnBalance.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ische\Documents\Github\SESH\SESH\Structure\1 - Whole System\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8206280B-A0E3-4D6A-B4A4-102F5F46CB2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11700"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Working Out" sheetId="3" r:id="rId1"/>
@@ -16,10 +22,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Working Out'!$A$1:$C$136</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -205,13 +217,13 @@
     <t>Transfers &amp; Transformation In</t>
   </si>
   <si>
-    <t>Transfers, Transformation &amp; Losses</t>
+    <t>TTL*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -438,16 +450,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Good 3" xfId="7"/>
-    <cellStyle name="Good 4" xfId="3"/>
+    <cellStyle name="Good 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Good 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 13 3" xfId="1"/>
-    <cellStyle name="Normal 13 3 3" xfId="2"/>
-    <cellStyle name="Normal 35" xfId="6"/>
-    <cellStyle name="Normal 36" xfId="8"/>
-    <cellStyle name="Normal 37" xfId="9"/>
-    <cellStyle name="Normal 38" xfId="5"/>
-    <cellStyle name="Normal 39" xfId="4"/>
+    <cellStyle name="Normal 13 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 13 3 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 35" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 36" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 37" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 38" xfId="5" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 39" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -717,28 +729,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,7 +767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -773,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -792,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -811,7 +823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -830,7 +842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -849,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -868,7 +880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -887,7 +899,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -906,7 +918,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -925,7 +937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -944,7 +956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -963,7 +975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -982,7 +994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1001,7 +1013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1020,7 +1032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1039,7 +1051,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
@@ -1058,7 +1070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
@@ -1077,7 +1089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -1096,7 +1108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -1115,7 +1127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>49</v>
       </c>
@@ -1127,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>49</v>
       </c>
@@ -1139,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
@@ -1151,7 +1163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
@@ -1163,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1175,7 +1187,7 @@
         <v>11953.572632683819</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
@@ -1187,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1199,7 +1211,7 @@
         <v>2967.9976667947853</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
@@ -1211,7 +1223,7 @@
         <v>6710.5260209438939</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
@@ -1223,7 +1235,7 @@
         <v>972.4461777555448</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -1235,7 +1247,7 @@
         <v>11650.208054151652</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>13</v>
       </c>
@@ -1247,7 +1259,7 @@
         <v>1038.9119930141237</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>357.81481657388258</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>13</v>
       </c>
@@ -1271,7 +1283,7 @@
         <v>263.24567172082999</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>13</v>
       </c>
@@ -1283,7 +1295,7 @@
         <v>4376.0488430404521</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>13</v>
       </c>
@@ -1295,7 +1307,7 @@
         <v>268.09599756874275</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
@@ -1307,7 +1319,7 @@
         <v>593.66732290216498</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -1319,7 +1331,7 @@
         <v>24954.6563307059</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -1331,7 +1343,7 @@
         <v>14091.653365434298</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>54</v>
       </c>
@@ -1343,7 +1355,7 @@
         <v>30219.38193800786</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>58</v>
       </c>
@@ -1355,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>54</v>
       </c>
@@ -1367,7 +1379,7 @@
         <v>60.93324677558072</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>54</v>
       </c>
@@ -1379,7 +1391,7 @@
         <v>895.70385173293903</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>54</v>
       </c>
@@ -1392,7 +1404,7 @@
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>54</v>
       </c>
@@ -1405,7 +1417,7 @@
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>54</v>
       </c>
@@ -1417,7 +1429,7 @@
         <v>853.86957673520146</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>54</v>
       </c>
@@ -1429,7 +1441,7 @@
         <v>4578.6809905426071</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -1441,7 +1453,7 @@
         <v>845.39852171455186</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -1453,7 +1465,7 @@
         <v>227.33523256795777</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>56</v>
       </c>
@@ -1465,7 +1477,7 @@
         <v>28.201536535983525</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -1477,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
@@ -1489,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>56</v>
       </c>
@@ -1501,7 +1513,7 @@
         <v>79.380273003241854</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
@@ -1513,7 +1525,7 @@
         <v>151.39981736084357</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>56</v>
       </c>
@@ -1525,7 +1537,7 @@
         <v>68.122607640065851</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>56</v>
       </c>
@@ -1537,7 +1549,7 @@
         <v>120.93006268598701</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
@@ -1549,7 +1561,7 @@
         <v>624.70011117190791</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>46</v>
       </c>
@@ -1561,7 +1573,7 @@
         <v>5786.0209006781306</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>47</v>
       </c>
@@ -1573,7 +1585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>16</v>
       </c>
@@ -1585,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -1597,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>16</v>
       </c>
@@ -1609,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>16</v>
       </c>
@@ -1621,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>16</v>
       </c>
@@ -1633,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>16</v>
       </c>
@@ -1645,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>16</v>
       </c>
@@ -1657,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>16</v>
       </c>
@@ -1669,7 +1681,7 @@
         <v>5786.0209006781306</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>46</v>
       </c>
@@ -1681,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>47</v>
       </c>
@@ -1693,7 +1705,7 @@
         <v>119.63693035253721</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>17</v>
       </c>
@@ -1705,7 +1717,7 @@
         <v>1226.1036973344865</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>58</v>
       </c>
@@ -1717,7 +1729,7 @@
         <v>4185.5311999527758</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>17</v>
       </c>
@@ -1729,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>17</v>
       </c>
@@ -1741,7 +1753,7 @@
         <v>730.47154133671813</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>17</v>
       </c>
@@ -1753,7 +1765,7 @@
         <v>1090.4646125001088</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>17</v>
       </c>
@@ -1765,7 +1777,7 @@
         <v>37.716437475378008</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>17</v>
       </c>
@@ -1777,7 +1789,7 @@
         <v>771.63008638802933</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>17</v>
       </c>
@@ -1789,7 +1801,7 @@
         <v>455.85862543396365</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>46</v>
       </c>
@@ -1801,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>47</v>
       </c>
@@ -1813,7 +1825,7 @@
         <v>119.63693035253721</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>57</v>
       </c>
@@ -1825,7 +1837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>58</v>
       </c>
@@ -1837,7 +1849,7 @@
         <v>121.41584435849438</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>57</v>
       </c>
@@ -1849,7 +1861,7 @@
         <v>61.272933863648511</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>57</v>
       </c>
@@ -1861,7 +1873,7 @@
         <v>9.8974895872053352</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>57</v>
       </c>
@@ -1873,7 +1885,7 @@
         <v>24.494109492182364</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>57</v>
       </c>
@@ -1885,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>57</v>
       </c>
@@ -1897,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>57</v>
       </c>
@@ -1909,7 +1921,7 @@
         <v>25.751311415458161</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>58</v>
       </c>
@@ -1920,77 +1932,77 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="24"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="24"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="24"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="24"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="24"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="24"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="5"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C128" s="5"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="5"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="5"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="5"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="5"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C136"/>
+  <autoFilter ref="A1:C136" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" style="4" customWidth="1"/>
-    <col min="2" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" style="4" customWidth="1"/>
+    <col min="2" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2845,14 +2857,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="A21:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2899,7 +2911,7 @@
       </c>
       <c r="B5" t="str">
         <f>'Working Out'!I5</f>
-        <v>Transfers, Transformation &amp; Losses</v>
+        <v>TTL*</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3058,16 +3070,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A88" sqref="A88:C166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3078,7 +3090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>VLOOKUP('Working Out'!A2,'Working Out'!$I:$J,2,0)</f>
         <v>0</v>
@@ -3092,7 +3104,7 @@
         <v>507.44028852584307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>VLOOKUP('Working Out'!A3,'Working Out'!$I:$J,2,0)</f>
         <v>1</v>
@@ -3106,7 +3118,7 @@
         <v>8.7004155918601298E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>VLOOKUP('Working Out'!A4,'Working Out'!$I:$J,2,0)</f>
         <v>11</v>
@@ -3120,7 +3132,7 @@
         <v>365.33074165217158</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>VLOOKUP('Working Out'!A5,'Working Out'!$I:$J,2,0)</f>
         <v>4</v>
@@ -3134,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>VLOOKUP('Working Out'!A6,'Working Out'!$I:$J,2,0)</f>
         <v>11</v>
@@ -3148,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>VLOOKUP('Working Out'!A7,'Working Out'!$I:$J,2,0)</f>
         <v>11</v>
@@ -3162,7 +3174,7 @@
         <v>93.280083568398254</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>VLOOKUP('Working Out'!A8,'Working Out'!$I:$J,2,0)</f>
         <v>11</v>
@@ -3176,7 +3188,7 @@
         <v>45.931319073176653</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>VLOOKUP('Working Out'!A9,'Working Out'!$I:$J,2,0)</f>
         <v>11</v>
@@ -3190,7 +3202,7 @@
         <v>0.32053293805785971</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>VLOOKUP('Working Out'!A10,'Working Out'!$I:$J,2,0)</f>
         <v>11</v>
@@ -3204,7 +3216,7 @@
         <v>2.5776199944543379</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>VLOOKUP('Working Out'!A11,'Working Out'!$I:$J,2,0)</f>
         <v>5</v>
@@ -3218,7 +3230,7 @@
         <v>1161.1181736533529</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>VLOOKUP('Working Out'!A12,'Working Out'!$I:$J,2,0)</f>
         <v>6</v>
@@ -3232,7 +3244,7 @@
         <v>2166.5480558023851</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>VLOOKUP('Working Out'!A13,'Working Out'!$I:$J,2,0)</f>
         <v>7</v>
@@ -3246,7 +3258,7 @@
         <v>4013.3616070159369</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>VLOOKUP('Working Out'!A14,'Working Out'!$I:$J,2,0)</f>
         <v>8</v>
@@ -3260,7 +3272,7 @@
         <v>4482.2084210939547</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>VLOOKUP('Working Out'!A15,'Working Out'!$I:$J,2,0)</f>
         <v>9</v>
@@ -3274,7 +3286,7 @@
         <v>2017.1033433724147</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>VLOOKUP('Working Out'!A16,'Working Out'!$I:$J,2,0)</f>
         <v>0</v>
@@ -3288,7 +3300,7 @@
         <v>48589.840699024528</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>VLOOKUP('Working Out'!A17,'Working Out'!$I:$J,2,0)</f>
         <v>1</v>
@@ -3302,7 +3314,7 @@
         <v>5377.4142107157004</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>VLOOKUP('Working Out'!A18,'Working Out'!$I:$J,2,0)</f>
         <v>12</v>
@@ -3316,7 +3328,7 @@
         <v>42065.105302522512</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>VLOOKUP('Working Out'!A19,'Working Out'!$I:$J,2,0)</f>
         <v>4</v>
@@ -3330,7 +3342,7 @@
         <v>51.437059283466994</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>VLOOKUP('Working Out'!A20,'Working Out'!$I:$J,2,0)</f>
         <v>12</v>
@@ -3344,7 +3356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>VLOOKUP('Working Out'!A21,'Working Out'!$I:$J,2,0)</f>
         <v>12</v>
@@ -3358,7 +3370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>VLOOKUP('Working Out'!A22,'Working Out'!$I:$J,2,0)</f>
         <v>12</v>
@@ -3372,7 +3384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>VLOOKUP('Working Out'!A23,'Working Out'!$I:$J,2,0)</f>
         <v>12</v>
@@ -3386,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>VLOOKUP('Working Out'!A24,'Working Out'!$I:$J,2,0)</f>
         <v>12</v>
@@ -3400,7 +3412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>VLOOKUP('Working Out'!A25,'Working Out'!$I:$J,2,0)</f>
         <v>12</v>
@@ -3414,7 +3426,7 @@
         <v>11953.572632683819</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>VLOOKUP('Working Out'!A26,'Working Out'!$I:$J,2,0)</f>
         <v>0</v>
@@ -3428,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>VLOOKUP('Working Out'!A27,'Working Out'!$I:$J,2,0)</f>
         <v>1</v>
@@ -3442,7 +3454,7 @@
         <v>2967.9976667947853</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>VLOOKUP('Working Out'!A28,'Working Out'!$I:$J,2,0)</f>
         <v>13</v>
@@ -3456,7 +3468,7 @@
         <v>6710.5260209438939</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>VLOOKUP('Working Out'!A29,'Working Out'!$I:$J,2,0)</f>
         <v>13</v>
@@ -3470,7 +3482,7 @@
         <v>972.4461777555448</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>VLOOKUP('Working Out'!A30,'Working Out'!$I:$J,2,0)</f>
         <v>4</v>
@@ -3484,7 +3496,7 @@
         <v>11650.208054151652</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>VLOOKUP('Working Out'!A31,'Working Out'!$I:$J,2,0)</f>
         <v>13</v>
@@ -3498,7 +3510,7 @@
         <v>1038.9119930141237</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>VLOOKUP('Working Out'!A32,'Working Out'!$I:$J,2,0)</f>
         <v>13</v>
@@ -3512,7 +3524,7 @@
         <v>357.81481657388258</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>VLOOKUP('Working Out'!A33,'Working Out'!$I:$J,2,0)</f>
         <v>13</v>
@@ -3526,7 +3538,7 @@
         <v>263.24567172082999</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>VLOOKUP('Working Out'!A34,'Working Out'!$I:$J,2,0)</f>
         <v>13</v>
@@ -3540,7 +3552,7 @@
         <v>4376.0488430404521</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>VLOOKUP('Working Out'!A35,'Working Out'!$I:$J,2,0)</f>
         <v>13</v>
@@ -3554,7 +3566,7 @@
         <v>268.09599756874275</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>VLOOKUP('Working Out'!A36,'Working Out'!$I:$J,2,0)</f>
         <v>13</v>
@@ -3568,7 +3580,7 @@
         <v>593.66732290216498</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>VLOOKUP('Working Out'!A37,'Working Out'!$I:$J,2,0)</f>
         <v>0</v>
@@ -3582,7 +3594,7 @@
         <v>24954.6563307059</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>VLOOKUP('Working Out'!A38,'Working Out'!$I:$J,2,0)</f>
         <v>1</v>
@@ -3596,7 +3608,7 @@
         <v>14091.653365434298</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>VLOOKUP('Working Out'!A39,'Working Out'!$I:$J,2,0)</f>
         <v>14</v>
@@ -3610,7 +3622,7 @@
         <v>30219.38193800786</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>VLOOKUP('Working Out'!A40,'Working Out'!$I:$J,2,0)</f>
         <v>4</v>
@@ -3624,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>VLOOKUP('Working Out'!A41,'Working Out'!$I:$J,2,0)</f>
         <v>14</v>
@@ -3638,7 +3650,7 @@
         <v>60.93324677558072</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>VLOOKUP('Working Out'!A42,'Working Out'!$I:$J,2,0)</f>
         <v>14</v>
@@ -3652,7 +3664,7 @@
         <v>895.70385173293903</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>VLOOKUP('Working Out'!A43,'Working Out'!$I:$J,2,0)</f>
         <v>14</v>
@@ -3666,7 +3678,7 @@
         <v>2437.826076868796</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>VLOOKUP('Working Out'!A44,'Working Out'!$I:$J,2,0)</f>
         <v>14</v>
@@ -3680,7 +3692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>VLOOKUP('Working Out'!A45,'Working Out'!$I:$J,2,0)</f>
         <v>14</v>
@@ -3694,7 +3706,7 @@
         <v>853.86957673520146</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>VLOOKUP('Working Out'!A46,'Working Out'!$I:$J,2,0)</f>
         <v>14</v>
@@ -3708,7 +3720,7 @@
         <v>4578.6809905426071</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>VLOOKUP('Working Out'!A47,'Working Out'!$I:$J,2,0)</f>
         <v>0</v>
@@ -3722,7 +3734,7 @@
         <v>845.39852171455186</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <f>VLOOKUP('Working Out'!A48,'Working Out'!$I:$J,2,0)</f>
         <v>1</v>
@@ -3736,7 +3748,7 @@
         <v>227.33523256795777</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <f>VLOOKUP('Working Out'!A49,'Working Out'!$I:$J,2,0)</f>
         <v>15</v>
@@ -3750,7 +3762,7 @@
         <v>28.201536535983525</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>VLOOKUP('Working Out'!A50,'Working Out'!$I:$J,2,0)</f>
         <v>4</v>
@@ -3764,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <f>VLOOKUP('Working Out'!A51,'Working Out'!$I:$J,2,0)</f>
         <v>15</v>
@@ -3778,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <f>VLOOKUP('Working Out'!A52,'Working Out'!$I:$J,2,0)</f>
         <v>15</v>
@@ -3792,7 +3804,7 @@
         <v>79.380273003241854</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <f>VLOOKUP('Working Out'!A53,'Working Out'!$I:$J,2,0)</f>
         <v>15</v>
@@ -3806,7 +3818,7 @@
         <v>151.39981736084357</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <f>VLOOKUP('Working Out'!A54,'Working Out'!$I:$J,2,0)</f>
         <v>15</v>
@@ -3820,7 +3832,7 @@
         <v>68.122607640065851</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <f>VLOOKUP('Working Out'!A55,'Working Out'!$I:$J,2,0)</f>
         <v>15</v>
@@ -3834,7 +3846,7 @@
         <v>120.93006268598701</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>VLOOKUP('Working Out'!A56,'Working Out'!$I:$J,2,0)</f>
         <v>15</v>
@@ -3848,7 +3860,7 @@
         <v>624.70011117190791</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <f>VLOOKUP('Working Out'!A57,'Working Out'!$I:$J,2,0)</f>
         <v>0</v>
@@ -3862,7 +3874,7 @@
         <v>5786.0209006781306</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <f>VLOOKUP('Working Out'!A58,'Working Out'!$I:$J,2,0)</f>
         <v>1</v>
@@ -3876,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <f>VLOOKUP('Working Out'!A59,'Working Out'!$I:$J,2,0)</f>
         <v>16</v>
@@ -3890,7 +3902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <f>VLOOKUP('Working Out'!A60,'Working Out'!$I:$J,2,0)</f>
         <v>4</v>
@@ -3904,7 +3916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <f>VLOOKUP('Working Out'!A61,'Working Out'!$I:$J,2,0)</f>
         <v>16</v>
@@ -3918,7 +3930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <f>VLOOKUP('Working Out'!A62,'Working Out'!$I:$J,2,0)</f>
         <v>16</v>
@@ -3932,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <f>VLOOKUP('Working Out'!A63,'Working Out'!$I:$J,2,0)</f>
         <v>16</v>
@@ -3946,7 +3958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <f>VLOOKUP('Working Out'!A64,'Working Out'!$I:$J,2,0)</f>
         <v>16</v>
@@ -3960,7 +3972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <f>VLOOKUP('Working Out'!A65,'Working Out'!$I:$J,2,0)</f>
         <v>16</v>
@@ -3974,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <f>VLOOKUP('Working Out'!A66,'Working Out'!$I:$J,2,0)</f>
         <v>16</v>
@@ -3988,7 +4000,7 @@
         <v>5786.0209006781306</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <f>VLOOKUP('Working Out'!A67,'Working Out'!$I:$J,2,0)</f>
         <v>0</v>
@@ -4002,7 +4014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <f>VLOOKUP('Working Out'!A68,'Working Out'!$I:$J,2,0)</f>
         <v>1</v>
@@ -4016,7 +4028,7 @@
         <v>119.63693035253721</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <f>VLOOKUP('Working Out'!A69,'Working Out'!$I:$J,2,0)</f>
         <v>17</v>
@@ -4030,7 +4042,7 @@
         <v>1226.1036973344865</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <f>VLOOKUP('Working Out'!A70,'Working Out'!$I:$J,2,0)</f>
         <v>4</v>
@@ -4044,7 +4056,7 @@
         <v>4185.5311999527758</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <f>VLOOKUP('Working Out'!A71,'Working Out'!$I:$J,2,0)</f>
         <v>17</v>
@@ -4058,7 +4070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <f>VLOOKUP('Working Out'!A72,'Working Out'!$I:$J,2,0)</f>
         <v>17</v>
@@ -4072,7 +4084,7 @@
         <v>730.47154133671813</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <f>VLOOKUP('Working Out'!A73,'Working Out'!$I:$J,2,0)</f>
         <v>17</v>
@@ -4086,7 +4098,7 @@
         <v>1090.4646125001088</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <f>VLOOKUP('Working Out'!A74,'Working Out'!$I:$J,2,0)</f>
         <v>17</v>
@@ -4100,7 +4112,7 @@
         <v>37.716437475378008</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <f>VLOOKUP('Working Out'!A75,'Working Out'!$I:$J,2,0)</f>
         <v>17</v>
@@ -4114,7 +4126,7 @@
         <v>771.63008638802933</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <f>VLOOKUP('Working Out'!A76,'Working Out'!$I:$J,2,0)</f>
         <v>17</v>
@@ -4128,7 +4140,7 @@
         <v>455.85862543396365</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <f>VLOOKUP('Working Out'!A77,'Working Out'!$I:$J,2,0)</f>
         <v>0</v>
@@ -4142,7 +4154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <f>VLOOKUP('Working Out'!A78,'Working Out'!$I:$J,2,0)</f>
         <v>1</v>
@@ -4156,7 +4168,7 @@
         <v>119.63693035253721</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <f>VLOOKUP('Working Out'!A79,'Working Out'!$I:$J,2,0)</f>
         <v>18</v>
@@ -4170,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <f>VLOOKUP('Working Out'!A80,'Working Out'!$I:$J,2,0)</f>
         <v>4</v>
@@ -4184,7 +4196,7 @@
         <v>121.41584435849438</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <f>VLOOKUP('Working Out'!A81,'Working Out'!$I:$J,2,0)</f>
         <v>18</v>
@@ -4198,7 +4210,7 @@
         <v>61.272933863648511</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <f>VLOOKUP('Working Out'!A82,'Working Out'!$I:$J,2,0)</f>
         <v>18</v>
@@ -4212,7 +4224,7 @@
         <v>9.8974895872053352</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <f>VLOOKUP('Working Out'!A83,'Working Out'!$I:$J,2,0)</f>
         <v>18</v>
@@ -4226,7 +4238,7 @@
         <v>24.494109492182364</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <f>VLOOKUP('Working Out'!A84,'Working Out'!$I:$J,2,0)</f>
         <v>18</v>
@@ -4240,7 +4252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <f>VLOOKUP('Working Out'!A85,'Working Out'!$I:$J,2,0)</f>
         <v>18</v>
@@ -4254,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <f>VLOOKUP('Working Out'!A86,'Working Out'!$I:$J,2,0)</f>
         <v>18</v>
@@ -4268,7 +4280,7 @@
         <v>25.751311415458161</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <f>VLOOKUP('Working Out'!A87,'Working Out'!$I:$J,2,0)</f>
         <v>4</v>
@@ -4288,21 +4300,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J141"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="9" max="9" width="26.44140625" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -4337,7 +4349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -4356,7 +4368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -4375,7 +4387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -4394,7 +4406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -4413,7 +4425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -4432,7 +4444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -4451,7 +4463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -4470,7 +4482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -4489,7 +4501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -4508,7 +4520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -4527,7 +4539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -4546,7 +4558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -4565,7 +4577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -4584,7 +4596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -4603,7 +4615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -4622,7 +4634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -4641,7 +4653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
@@ -4660,7 +4672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -4679,7 +4691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
@@ -4698,7 +4710,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>49</v>
       </c>
@@ -4717,7 +4729,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
@@ -4736,7 +4748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
@@ -4755,7 +4767,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -4774,7 +4786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
@@ -4793,7 +4805,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -4805,7 +4817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -4817,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -4829,7 +4841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -4841,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -4853,7 +4865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
@@ -4865,7 +4877,7 @@
         <v>2559.5052509966904</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
@@ -4877,7 +4889,7 @@
         <v>9394.0673816871295</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -4889,7 +4901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -4901,7 +4913,7 @@
         <v>2967.9976667947853</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>13</v>
       </c>
@@ -4913,7 +4925,7 @@
         <v>6710.5260209438939</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
@@ -4925,7 +4937,7 @@
         <v>972.4461777555448</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -4937,7 +4949,7 @@
         <v>19.073019937128301</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>13</v>
       </c>
@@ -4949,7 +4961,7 @@
         <v>1038.9119930141237</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>13</v>
       </c>
@@ -4961,7 +4973,7 @@
         <v>357.81481657388258</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>13</v>
       </c>
@@ -4973,7 +4985,7 @@
         <v>263.24567172082999</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>13</v>
       </c>
@@ -4985,7 +4997,7 @@
         <v>4376.0488430404521</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>13</v>
       </c>
@@ -4998,7 +5010,7 @@
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -5011,7 +5023,7 @@
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
@@ -5023,7 +5035,7 @@
         <v>357.81481657388258</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
@@ -5035,7 +5047,7 @@
         <v>263.24567172082999</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
@@ -5047,7 +5059,7 @@
         <v>4376.0488430404521</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>11</v>
       </c>
@@ -5059,7 +5071,7 @@
         <v>268.09599756874275</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -5071,7 +5083,7 @@
         <v>2559.5052509966904</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -5083,7 +5095,7 @@
         <v>9071.6297832178334</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>13</v>
       </c>
@@ -5095,7 +5107,7 @@
         <v>592.27299800725962</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>46</v>
       </c>
@@ -5107,7 +5119,7 @@
         <v>24954.6563307059</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>47</v>
       </c>
@@ -5119,7 +5131,7 @@
         <v>14091.653365434298</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
@@ -5131,7 +5143,7 @@
         <v>30219.38193800786</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>14</v>
       </c>
@@ -5143,7 +5155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
@@ -5155,7 +5167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>54</v>
       </c>
@@ -5167,7 +5179,7 @@
         <v>60.93324677558072</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>54</v>
       </c>
@@ -5179,7 +5191,7 @@
         <v>895.70385173293903</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>54</v>
       </c>
@@ -5191,7 +5203,7 @@
         <v>2437.826076868796</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>54</v>
       </c>
@@ -5203,7 +5215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>54</v>
       </c>
@@ -5215,7 +5227,7 @@
         <v>853.86957673520146</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -5227,7 +5239,7 @@
         <v>60.93324677558072</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
@@ -5239,7 +5251,7 @@
         <v>895.70385173293903</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>9</v>
       </c>
@@ -5251,7 +5263,7 @@
         <v>2437.826076868796</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
@@ -5263,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>11</v>
       </c>
@@ -5275,7 +5287,7 @@
         <v>853.86957673520146</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>52</v>
       </c>
@@ -5287,7 +5299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>54</v>
       </c>
@@ -5299,7 +5311,7 @@
         <v>962.87537035222795</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>54</v>
       </c>
@@ -5311,7 +5323,7 @@
         <v>3615.8056201903792</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>46</v>
       </c>
@@ -5323,7 +5335,7 @@
         <v>845.39852171455186</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>47</v>
       </c>
@@ -5335,7 +5347,7 @@
         <v>227.33523256795777</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>56</v>
       </c>
@@ -5347,7 +5359,7 @@
         <v>28.201536535983525</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>14</v>
       </c>
@@ -5359,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>48</v>
       </c>
@@ -5371,7 +5383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>56</v>
       </c>
@@ -5383,7 +5395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>56</v>
       </c>
@@ -5395,7 +5407,7 @@
         <v>79.380273003241854</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>56</v>
       </c>
@@ -5407,7 +5419,7 @@
         <v>151.39981736084357</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>56</v>
       </c>
@@ -5419,7 +5431,7 @@
         <v>68.122607640065851</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>56</v>
       </c>
@@ -5431,7 +5443,7 @@
         <v>120.93006268598701</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -5443,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>8</v>
       </c>
@@ -5455,7 +5467,7 @@
         <v>79.380273003241854</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>9</v>
       </c>
@@ -5467,7 +5479,7 @@
         <v>151.39981736084357</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>10</v>
       </c>
@@ -5479,7 +5491,7 @@
         <v>68.122607640065851</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>11</v>
       </c>
@@ -5491,7 +5503,7 @@
         <v>120.93006268598701</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>52</v>
       </c>
@@ -5503,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>56</v>
       </c>
@@ -5515,7 +5527,7 @@
         <v>624.70011117190791</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>56</v>
       </c>
@@ -5527,7 +5539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>46</v>
       </c>
@@ -5539,7 +5551,7 @@
         <v>5786.0209006781306</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>47</v>
       </c>
@@ -5551,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>16</v>
       </c>
@@ -5563,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>14</v>
       </c>
@@ -5575,7 +5587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>48</v>
       </c>
@@ -5587,7 +5599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>16</v>
       </c>
@@ -5599,7 +5611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>16</v>
       </c>
@@ -5611,7 +5623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>16</v>
       </c>
@@ -5623,7 +5635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>16</v>
       </c>
@@ -5635,7 +5647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>16</v>
       </c>
@@ -5647,7 +5659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>7</v>
       </c>
@@ -5659,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>8</v>
       </c>
@@ -5671,7 +5683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>9</v>
       </c>
@@ -5683,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>10</v>
       </c>
@@ -5695,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>11</v>
       </c>
@@ -5707,7 +5719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>16</v>
       </c>
@@ -5719,7 +5731,7 @@
         <v>1952.9624355017334</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>16</v>
       </c>
@@ -5731,7 +5743,7 @@
         <v>3833.0584651763975</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>16</v>
       </c>
@@ -5743,7 +5755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>46</v>
       </c>
@@ -5755,7 +5767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>47</v>
       </c>
@@ -5767,7 +5779,7 @@
         <v>119.63693035253721</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>17</v>
       </c>
@@ -5779,7 +5791,7 @@
         <v>1226.1036973344865</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>14</v>
       </c>
@@ -5791,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>48</v>
       </c>
@@ -5803,7 +5815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>17</v>
       </c>
@@ -5815,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>17</v>
       </c>
@@ -5827,7 +5839,7 @@
         <v>730.47154133671813</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>17</v>
       </c>
@@ -5839,7 +5851,7 @@
         <v>1090.4646125001088</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>17</v>
       </c>
@@ -5851,7 +5863,7 @@
         <v>37.716437475378008</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>17</v>
       </c>
@@ -5863,7 +5875,7 @@
         <v>771.63008638802933</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>7</v>
       </c>
@@ -5875,7 +5887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>8</v>
       </c>
@@ -5887,7 +5899,7 @@
         <v>730.47154133671813</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>9</v>
       </c>
@@ -5899,7 +5911,7 @@
         <v>1090.4646125001088</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>10</v>
       </c>
@@ -5911,7 +5923,7 @@
         <v>37.716437475378008</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>11</v>
       </c>
@@ -5923,7 +5935,7 @@
         <v>771.63008638802933</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>52</v>
       </c>
@@ -5935,7 +5947,7 @@
         <v>1952.9624355017334</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>53</v>
       </c>
@@ -5947,7 +5959,7 @@
         <v>2232.5687644510422</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>17</v>
       </c>
@@ -5959,7 +5971,7 @@
         <v>455.85862543396365</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>46</v>
       </c>
@@ -5971,7 +5983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>47</v>
       </c>
@@ -5983,7 +5995,7 @@
         <v>119.63693035253721</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>57</v>
       </c>
@@ -5995,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>14</v>
       </c>
@@ -6007,7 +6019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -6019,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>57</v>
       </c>
@@ -6031,7 +6043,7 @@
         <v>61.272933863648511</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>57</v>
       </c>
@@ -6043,7 +6055,7 @@
         <v>9.8974895872053352</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>57</v>
       </c>
@@ -6055,7 +6067,7 @@
         <v>24.494109492182364</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>57</v>
       </c>
@@ -6067,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>57</v>
       </c>
@@ -6079,7 +6091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>7</v>
       </c>
@@ -6091,7 +6103,7 @@
         <v>61.272933863648511</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>8</v>
       </c>
@@ -6103,7 +6115,7 @@
         <v>9.8974895872053352</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -6115,7 +6127,7 @@
         <v>24.494109492182364</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>10</v>
       </c>
@@ -6127,7 +6139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>11</v>
       </c>
@@ -6139,7 +6151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>52</v>
       </c>
@@ -6151,7 +6163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>53</v>
       </c>
@@ -6163,7 +6175,7 @@
         <v>121.41584435849438</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>57</v>
       </c>

</xml_diff>